<commit_message>
Se suben correcciones y nuevas paginas
</commit_message>
<xml_diff>
--- a/Spring2_Consultas/FRONT Relacion de pantallas.xlsx
+++ b/Spring2_Consultas/FRONT Relacion de pantallas.xlsx
@@ -252,7 +252,7 @@
     <t xml:space="preserve">José</t>
   </si>
   <si>
-    <t xml:space="preserve">Posicion Mesa de dinero </t>
+    <t xml:space="preserve">Posicion Mesa de dinero  (2 Grids)</t>
   </si>
   <si>
     <t xml:space="preserve">E.	Posición  mesa de dinero </t>
@@ -461,7 +461,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> (Cancelacion de envio de Edo cuenta Fisico)</t>
+      <t xml:space="preserve"> (Cancelacion de envio de Edo cuenta Fisico) (puros combos) (Falta pantalla Terminos y condiciones y su texto)</t>
     </r>
   </si>
   <si>
@@ -1005,7 +1005,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1070,14 +1070,14 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1094,7 +1094,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1369,26 +1373,26 @@
   </sheetPr>
   <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.25101214574899"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.1417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.81781376518219"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="90.9433198380567"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="91.6923076923077"/>
     <col collapsed="false" hidden="false" max="30" min="14" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="31" style="0" width="12.8542510121458"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1659,10 +1663,10 @@
       <c r="A7" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1715,7 +1719,7 @@
       <c r="A8" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="17" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1811,7 +1815,7 @@
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <v>6</v>
       </c>
@@ -2023,11 +2027,11 @@
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -2075,11 +2079,11 @@
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="23" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -2133,14 +2137,14 @@
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <v>12</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>70</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -2185,14 +2189,14 @@
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
         <v>13</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -2202,7 +2206,7 @@
         <v>38</v>
       </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13" t="s">
         <v>33</v>
@@ -2237,14 +2241,14 @@
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>77</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -2256,7 +2260,7 @@
       <c r="F18" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G18" s="23"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13" t="s">
         <v>33</v>
@@ -2293,16 +2297,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="17"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="7"/>
       <c r="E19" s="18"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="J19" s="14"/>
-      <c r="K19" s="25" t="n">
+      <c r="K19" s="26" t="n">
         <f aca="false">SUM(K5:K18)</f>
         <v>313</v>
       </c>
@@ -2328,32 +2332,32 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="27" t="s">
+      <c r="B20" s="27"/>
+      <c r="C20" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -2377,17 +2381,17 @@
       <c r="B21" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="35"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="36" t="n">
+      <c r="F21" s="37" t="n">
         <v>10</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="24" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="10" t="s">
@@ -2424,17 +2428,17 @@
       <c r="B22" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="7" t="s">
         <v>90</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="36" t="n">
+      <c r="F22" s="37" t="n">
         <v>12</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="24" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="10" t="s">
@@ -2442,7 +2446,7 @@
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
-      <c r="L22" s="23"/>
+      <c r="L22" s="24"/>
       <c r="M22" s="14" t="s">
         <v>93</v>
       </c>
@@ -2471,17 +2475,17 @@
       <c r="B23" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="35"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="7" t="s">
         <v>95</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="36" t="n">
+      <c r="F23" s="37" t="n">
         <v>15</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="24" t="s">
         <v>20</v>
       </c>
       <c r="H23" s="10"/>
@@ -2511,26 +2515,26 @@
       <c r="A24" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="7" t="s">
         <v>95</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F24" s="36" t="n">
+      <c r="F24" s="37" t="n">
         <v>15</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="24" t="s">
         <v>53</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
-      <c r="L24" s="38"/>
+      <c r="L24" s="39"/>
       <c r="M24" s="14" t="n">
         <v>40</v>
       </c>
@@ -2559,22 +2563,22 @@
       <c r="B25" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="35"/>
+      <c r="C25" s="36"/>
       <c r="D25" s="7" t="s">
         <v>95</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="36" t="n">
+      <c r="F25" s="37" t="n">
         <v>15</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G25" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
       <c r="L25" s="13"/>
       <c r="M25" s="14"/>
       <c r="N25" s="2"/>
@@ -2602,23 +2606,23 @@
       <c r="B26" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="40"/>
+      <c r="C26" s="41"/>
       <c r="D26" s="7" t="s">
         <v>95</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F26" s="36" t="n">
+      <c r="F26" s="37" t="n">
         <v>15</v>
       </c>
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="L26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="L26" s="43"/>
       <c r="M26" s="14" t="n">
         <v>43</v>
       </c>
@@ -2644,26 +2648,26 @@
       <c r="A27" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44" t="s">
+      <c r="C27" s="45"/>
+      <c r="D27" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="E27" s="44" t="s">
+      <c r="E27" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="F27" s="45" t="n">
+      <c r="F27" s="46" t="n">
         <v>12</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="L27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="L27" s="48"/>
       <c r="M27" s="14" t="n">
         <v>44</v>
       </c>
@@ -2689,26 +2693,26 @@
       <c r="A28" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44" t="s">
+      <c r="C28" s="45"/>
+      <c r="D28" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="44" t="s">
+      <c r="E28" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="F28" s="45" t="n">
+      <c r="F28" s="46" t="n">
         <v>10</v>
       </c>
-      <c r="G28" s="36" t="s">
+      <c r="G28" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="H28" s="46"/>
-      <c r="I28" s="46"/>
-      <c r="J28" s="46"/>
-      <c r="L28" s="48"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="L28" s="49"/>
       <c r="M28" s="14" t="n">
         <v>74</v>
       </c>
@@ -2734,26 +2738,26 @@
       <c r="A29" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44" t="s">
+      <c r="C29" s="45"/>
+      <c r="D29" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="44" t="s">
+      <c r="E29" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="45" t="n">
+      <c r="F29" s="46" t="n">
         <v>24</v>
       </c>
-      <c r="G29" s="36" t="s">
+      <c r="G29" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="H29" s="47"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="L29" s="49"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="L29" s="50"/>
       <c r="M29" s="14" t="n">
         <v>76</v>
       </c>
@@ -2779,19 +2783,19 @@
       <c r="A30" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44" t="s">
+      <c r="C30" s="45"/>
+      <c r="D30" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="44"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="L30" s="49"/>
+      <c r="E30" s="45"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="L30" s="50"/>
       <c r="M30" s="14"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -2815,20 +2819,20 @@
       <c r="A31" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="43" t="s">
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="H31" s="47"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="50"/>
-      <c r="L31" s="50"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="51"/>
+      <c r="L31" s="51"/>
       <c r="M31" s="14" t="n">
         <v>45</v>
       </c>
@@ -2854,20 +2858,20 @@
       <c r="A32" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="43" t="s">
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="L32" s="47"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="L32" s="48"/>
       <c r="M32" s="14" t="n">
         <v>42</v>
       </c>
@@ -2893,20 +2897,20 @@
       <c r="A33" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="43" t="s">
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="L33" s="47"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="L33" s="48"/>
       <c r="M33" s="14" t="n">
         <v>38</v>
       </c>
@@ -2932,18 +2936,18 @@
       <c r="A34" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="B34" s="43"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="48"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
@@ -2964,18 +2968,18 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="48"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
@@ -2996,18 +3000,18 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="48"/>
+      <c r="L36" s="48"/>
+      <c r="M36" s="48"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
@@ -3028,18 +3032,18 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="47"/>
-      <c r="L37" s="47"/>
-      <c r="M37" s="47"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="48"/>
+      <c r="M37" s="48"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
@@ -3059,19 +3063,19 @@
       <c r="AD37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="51"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="54"/>
-      <c r="L38" s="54"/>
-      <c r="M38" s="54"/>
+      <c r="A38" s="52"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="55"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
@@ -3091,21 +3095,21 @@
       <c r="AD38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="51"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="57" t="n">
+      <c r="A39" s="52"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="58" t="n">
         <v>104</v>
       </c>
-      <c r="G39" s="55"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="54"/>
-      <c r="M39" s="54"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="55"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
@@ -3125,21 +3129,21 @@
       <c r="AD39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="58"/>
-      <c r="B40" s="59"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="54"/>
-      <c r="F40" s="45" t="s">
+      <c r="A40" s="59"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="G40" s="54"/>
-      <c r="H40" s="54"/>
-      <c r="I40" s="54"/>
-      <c r="J40" s="54"/>
-      <c r="K40" s="54"/>
-      <c r="L40" s="54"/>
-      <c r="M40" s="54"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="55"/>
+      <c r="I40" s="55"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="55"/>
+      <c r="M40" s="55"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
@@ -3196,342 +3200,342 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.8582995951417"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.9554655870445"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.2753036437247"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="2.46558704453441"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="27" min="9" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="12.8542510121458"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="G2" s="60" t="s">
+      <c r="D2" s="61"/>
+      <c r="G2" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="60"/>
+      <c r="H2" s="61"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="61"/>
-      <c r="C3" s="61" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61" t="s">
+      <c r="F3" s="62"/>
+      <c r="G3" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="62" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="62"/>
-      <c r="B4" s="63" t="n">
+      <c r="A4" s="63"/>
+      <c r="B4" s="64" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="F4" s="62" t="n">
+      <c r="D4" s="64"/>
+      <c r="F4" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="H4" s="63"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="63"/>
-      <c r="C5" s="65" t="s">
+      <c r="B5" s="64"/>
+      <c r="C5" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="63" t="n">
+      <c r="D5" s="64" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="62" t="n">
+      <c r="E5" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="H5" s="63" t="n">
+      <c r="H5" s="64" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="63" t="n">
+      <c r="B6" s="64" t="n">
         <f aca="false">D7+D8+D9+D10</f>
         <v>10</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="65" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="62" t="n">
+      <c r="D6" s="64"/>
+      <c r="E6" s="63" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="62" t="n">
+      <c r="F6" s="63" t="n">
         <v>3</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="H6" s="63"/>
+      <c r="H6" s="64"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="63"/>
-      <c r="C7" s="66" t="s">
+      <c r="B7" s="64"/>
+      <c r="C7" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="63" t="n">
+      <c r="D7" s="64" t="n">
         <v>3</v>
       </c>
-      <c r="E7" s="62"/>
-      <c r="G7" s="66" t="s">
+      <c r="E7" s="63"/>
+      <c r="G7" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="H7" s="63" t="n">
+      <c r="H7" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="63"/>
-      <c r="C8" s="66" t="s">
+      <c r="B8" s="64"/>
+      <c r="C8" s="67" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="63" t="n">
+      <c r="D8" s="64" t="n">
         <v>2</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">H9+H10+H11+H12</f>
         <v>9</v>
       </c>
-      <c r="G8" s="64" t="s">
+      <c r="G8" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="63"/>
+      <c r="H8" s="64"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="63"/>
-      <c r="C9" s="66" t="s">
+      <c r="B9" s="64"/>
+      <c r="C9" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="63" t="n">
+      <c r="D9" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="66" t="s">
+      <c r="G9" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="H9" s="63" t="n">
+      <c r="H9" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="63"/>
-      <c r="C10" s="66" t="s">
+      <c r="B10" s="64"/>
+      <c r="C10" s="67" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="63" t="n">
+      <c r="D10" s="64" t="n">
         <v>4</v>
       </c>
-      <c r="G10" s="66" t="s">
+      <c r="G10" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="H10" s="63" t="n">
+      <c r="H10" s="64" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="62"/>
-      <c r="B11" s="63" t="n">
+      <c r="A11" s="63"/>
+      <c r="B11" s="64" t="n">
         <v>3</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="62" t="n">
+      <c r="D11" s="64"/>
+      <c r="E11" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="66" t="s">
+      <c r="G11" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="H11" s="63" t="n">
+      <c r="H11" s="64" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="63"/>
-      <c r="C12" s="66" t="s">
+      <c r="B12" s="64"/>
+      <c r="C12" s="67" t="s">
         <v>128</v>
       </c>
-      <c r="D12" s="63" t="n">
+      <c r="D12" s="64" t="n">
         <v>3</v>
       </c>
-      <c r="G12" s="66" t="s">
+      <c r="G12" s="67" t="s">
         <v>126</v>
       </c>
-      <c r="H12" s="63" t="n">
+      <c r="H12" s="64" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="63" t="n">
+      <c r="B13" s="64" t="n">
         <f aca="false">D14+D15+D16+D17</f>
         <v>9</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="D13" s="63"/>
-      <c r="E13" s="62" t="n">
+      <c r="D13" s="64"/>
+      <c r="E13" s="63" t="n">
         <v>5</v>
       </c>
-      <c r="F13" s="62" t="n">
+      <c r="F13" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="G13" s="64" t="s">
+      <c r="G13" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="H13" s="63"/>
+      <c r="H13" s="64"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="63"/>
-      <c r="C14" s="66" t="s">
+      <c r="B14" s="64"/>
+      <c r="C14" s="67" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="63" t="n">
+      <c r="D14" s="64" t="n">
         <v>3</v>
       </c>
-      <c r="G14" s="66" t="s">
+      <c r="G14" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="H14" s="63" t="n">
+      <c r="H14" s="64" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="63"/>
-      <c r="C15" s="66" t="s">
+      <c r="B15" s="64"/>
+      <c r="C15" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="D15" s="63" t="n">
+      <c r="D15" s="64" t="n">
         <v>2</v>
       </c>
-      <c r="H15" s="63"/>
+      <c r="H15" s="64"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="63"/>
-      <c r="C16" s="66" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="D16" s="63" t="n">
+      <c r="D16" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="68" t="n">
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="69" t="n">
         <f aca="false">SUM(H4:H15)</f>
         <v>15</v>
       </c>
-      <c r="I16" s="62" t="s">
+      <c r="I16" s="63" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="63"/>
-      <c r="C17" s="66" t="s">
+      <c r="B17" s="64"/>
+      <c r="C17" s="67" t="s">
         <v>126</v>
       </c>
-      <c r="D17" s="63" t="n">
+      <c r="D17" s="64" t="n">
         <v>3</v>
       </c>
-      <c r="G17" s="66"/>
-      <c r="H17" s="62" t="n">
+      <c r="G17" s="67"/>
+      <c r="H17" s="63" t="n">
         <v>12</v>
       </c>
-      <c r="I17" s="62" t="s">
+      <c r="I17" s="63" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="62"/>
-      <c r="B18" s="63" t="n">
+      <c r="A18" s="63"/>
+      <c r="B18" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C18" s="64" t="s">
+      <c r="C18" s="65" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="63"/>
-      <c r="E18" s="62" t="n">
+      <c r="D18" s="64"/>
+      <c r="E18" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="G18" s="64"/>
-      <c r="H18" s="62" t="n">
+      <c r="G18" s="65"/>
+      <c r="H18" s="63" t="n">
         <v>10</v>
       </c>
-      <c r="I18" s="62" t="s">
+      <c r="I18" s="63" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="63"/>
-      <c r="C19" s="66" t="s">
+      <c r="B19" s="64"/>
+      <c r="C19" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="D19" s="63" t="n">
+      <c r="D19" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="G19" s="66"/>
+      <c r="G19" s="67"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="62"/>
-      <c r="B20" s="63" t="n">
+      <c r="A20" s="63"/>
+      <c r="B20" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="64" t="s">
+      <c r="C20" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="D20" s="63"/>
-      <c r="E20" s="62" t="n">
+      <c r="D20" s="64"/>
+      <c r="E20" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="G20" s="64"/>
+      <c r="G20" s="65"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="63"/>
-      <c r="C21" s="66" t="s">
+      <c r="B21" s="64"/>
+      <c r="C21" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="D21" s="63" t="n">
+      <c r="D21" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="66"/>
+      <c r="G21" s="67"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="63"/>
+      <c r="B22" s="64"/>
       <c r="E22" s="0" t="n">
         <f aca="false">SUM(E5:E21)</f>
         <v>13</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="69"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="70" t="n">
+      <c r="B23" s="70"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="71" t="n">
         <f aca="false">SUM(D4:D22)</f>
         <v>26</v>
       </c>
-      <c r="E23" s="62" t="s">
+      <c r="E23" s="63" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3564,7 +3568,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="26" min="1" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="12.8542510121458"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>